<commit_message>
Updated and corrected EC3 for Tella
</commit_message>
<xml_diff>
--- a/full_tool_evaluation_stylized.xlsx
+++ b/full_tool_evaluation_stylized.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amsuni-my.sharepoint.com/personal/james_bush_ii_student_uva_nl/Documents/thesis_final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2081AC4A-61C1-478F-B65F-5C13FE051C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{2081AC4A-61C1-478F-B65F-5C13FE051C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{996443BE-BC0F-41FE-9F1F-29355DD84D32}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{2FDC8EDD-81E5-40A6-9283-0E9D69291070}"/>
+    <workbookView xWindow="45" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{2FDC8EDD-81E5-40A6-9283-0E9D69291070}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,9 +116,6 @@
     <t>Offline capture with queue submissions once online (EC2.1);  * Form based collection when connected ODK (EC2.3)*; Mobile app (EC2.2);</t>
   </si>
   <si>
-    <t>Automatically encrypts photos, videos, and audio recordings; All data being transferred between Tella and servers is encrypted through Transport Layer Security (TLS) (EC3.1); Files are pin/password protected; Captures verified metadata including a hash (EC3.2); Camouflage mode, quick delete panic button;</t>
-  </si>
-  <si>
     <t>Democratization of data submission and organization</t>
   </si>
   <si>
@@ -683,6 +680,9 @@
   </si>
   <si>
     <t xml:space="preserve">USAID's Amazon Alive Activity, implemented by Chemonics, empowers indigenous communities in Colombia to monitor and safeguard their land, heritage, and rich biodiversity. Timby allows them to track and document potential threats to their territories, including illegal logging, mining, and land encroachment; while integrating their traditional knowledge, cultures, and ancestral ways of life and improving their decision-making processes (https://timby.org/case-studies/). </t>
+  </si>
+  <si>
+    <t>Automatically encrypts photos, videos, and audio recordings; All data being transferred between Tella and servers is encrypted through Transport Layer Security (TLS) (EC3.1); Files are pin/password protected; Captures verified metadata including a hash, but is not used to verify authenticity; Camouflage mode, quick delete panic button;</t>
   </si>
 </sst>
 </file>
@@ -1117,8 +1117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2F69AD-EFF9-4BE1-A80F-730B25438A05}">
   <dimension ref="C5:F174"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1142,7 +1142,7 @@
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="3:6" ht="144" x14ac:dyDescent="0.3">
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -1151,82 +1151,82 @@
       <c r="E7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C8" s="5"/>
+      <c r="C8" s="8"/>
       <c r="D8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C9" s="5"/>
+      <c r="C9" s="8"/>
       <c r="D9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="3:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="C10" s="5"/>
+      <c r="C10" s="8"/>
       <c r="D10" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C11" s="5"/>
+      <c r="C11" s="8"/>
       <c r="D11" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C12" s="5"/>
+      <c r="C12" s="8"/>
       <c r="D12" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="7"/>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C13" s="5"/>
+      <c r="C13" s="8"/>
       <c r="D13" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C14" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="8"/>
       <c r="D14" s="6" t="s">
         <v>19</v>
       </c>
@@ -1245,7 +1245,7 @@
       <c r="E15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1257,31 +1257,31 @@
       <c r="E16" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="3:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="C17" s="10"/>
       <c r="D17" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="18" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C18" s="10"/>
       <c r="D18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1291,9 +1291,9 @@
         <v>13</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1303,141 +1303,141 @@
         <v>15</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="21" spans="3:6" ht="144" x14ac:dyDescent="0.3">
       <c r="C21" s="10"/>
       <c r="D21" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F21" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C22" s="10"/>
       <c r="D22" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E22" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="C23" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="F22" s="9"/>
-    </row>
-    <row r="23" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C23" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="24" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C24" s="5"/>
+      <c r="C24" s="8"/>
       <c r="D24" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F24" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="25" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C25" s="5"/>
+      <c r="C25" s="8"/>
       <c r="D25" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E25" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C26" s="8"/>
+      <c r="D26" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F25" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C26" s="5"/>
-      <c r="D26" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="27" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C27" s="5"/>
+      <c r="C27" s="8"/>
       <c r="D27" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F27" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="28" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C28" s="5"/>
+      <c r="C28" s="8"/>
       <c r="D28" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E28" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="C29" s="8"/>
+      <c r="D29" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F28" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="3:6" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="C29" s="5"/>
-      <c r="D29" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C30" s="5"/>
+      <c r="F29" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C30" s="8"/>
       <c r="D30" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F30" s="9"/>
     </row>
     <row r="31" spans="3:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="C31" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F31" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1447,9 +1447,9 @@
         <v>24</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F32" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1459,21 +1459,21 @@
         <v>8</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F33" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="34" spans="3:6" ht="72" x14ac:dyDescent="0.3">
       <c r="C34" s="10"/>
       <c r="D34" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F34" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1483,9 +1483,9 @@
         <v>13</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F35" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1495,1005 +1495,1005 @@
         <v>15</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F36" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F36" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="37" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="C37" s="10"/>
       <c r="D37" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C38" s="10"/>
       <c r="D38" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E38" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="3:6" ht="144" x14ac:dyDescent="0.3">
+      <c r="C39" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="F38" s="9"/>
-    </row>
-    <row r="39" spans="3:6" ht="144" x14ac:dyDescent="0.3">
-      <c r="C39" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E39" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F39" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F39" s="8" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="40" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C40" s="5"/>
+      <c r="C40" s="8"/>
       <c r="D40" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F40" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F40" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="41" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C41" s="5"/>
+      <c r="C41" s="8"/>
       <c r="D41" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E41" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F41" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F41" s="8" t="s">
+    </row>
+    <row r="42" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C42" s="8"/>
+      <c r="D42" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E42" s="7" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="42" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C42" s="5"/>
-      <c r="D42" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F42" s="8" t="s">
+      <c r="F42" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="43" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C43" s="5"/>
+      <c r="C43" s="8"/>
       <c r="D43" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F43" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="44" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C44" s="5"/>
+      <c r="C44" s="8"/>
       <c r="D44" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E44" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C45" s="8"/>
+      <c r="D45" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E45" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F44" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C45" s="5"/>
-      <c r="D45" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E45" s="7" t="s">
+      <c r="F45" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F45" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="46" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C46" s="5"/>
+    </row>
+    <row r="46" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C46" s="8"/>
       <c r="D46" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E46" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F46" s="9"/>
+    </row>
+    <row r="47" spans="3:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="C47" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="F46" s="9"/>
-    </row>
-    <row r="47" spans="3:6" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C47" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F47" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F47" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="48" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C48" s="5"/>
+      <c r="C48" s="8"/>
       <c r="D48" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F48" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F48" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="49" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C49" s="5"/>
+      <c r="C49" s="8"/>
       <c r="D49" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E49" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C50" s="8"/>
+      <c r="D50" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E50" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F49" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C50" s="5"/>
-      <c r="D50" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F50" s="8" t="s">
+      <c r="F50" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="51" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C51" s="5"/>
+      <c r="C51" s="8"/>
       <c r="D51" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F51" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F51" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="52" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C52" s="5"/>
+      <c r="C52" s="8"/>
       <c r="D52" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E52" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="C53" s="8"/>
+      <c r="D53" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E53" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F52" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="53" spans="3:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="C53" s="5"/>
-      <c r="D53" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C54" s="5"/>
+      <c r="F53" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C54" s="8"/>
       <c r="D54" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E54" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F54" s="9"/>
+    </row>
+    <row r="55" spans="3:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="C55" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="F54" s="9"/>
-    </row>
-    <row r="55" spans="3:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="C55" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F55" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F55" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="56" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C56" s="5"/>
+      <c r="C56" s="8"/>
       <c r="D56" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E56" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F56" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="F56" s="8" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="57" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C57" s="5"/>
+      <c r="C57" s="8"/>
       <c r="D57" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E57" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F57" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="F57" s="8" t="s">
+    </row>
+    <row r="58" spans="3:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="C58" s="8"/>
+      <c r="D58" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E58" s="7" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="58" spans="3:6" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C58" s="5"/>
-      <c r="D58" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E58" s="7" t="s">
+      <c r="F58" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F58" s="8" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="59" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C59" s="5"/>
+      <c r="C59" s="8"/>
       <c r="D59" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="F59" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F59" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="60" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C60" s="5"/>
+      <c r="C60" s="8"/>
       <c r="D60" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E60" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="3:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="C61" s="8"/>
+      <c r="D61" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E61" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F60" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="61" spans="3:6" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C61" s="5"/>
-      <c r="D61" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F61" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="62" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C62" s="5"/>
+      <c r="F61" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C62" s="8"/>
       <c r="D62" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E62" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F62" s="9"/>
+    </row>
+    <row r="63" spans="3:6" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="C63" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="F62" s="9"/>
-    </row>
-    <row r="63" spans="3:6" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="C63" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F63" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F63" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="64" spans="3:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="C64" s="5"/>
+      <c r="C64" s="8"/>
       <c r="D64" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F64" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F64" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="65" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C65" s="5"/>
+      <c r="C65" s="8"/>
       <c r="D65" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E65" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="C66" s="8"/>
+      <c r="D66" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E66" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F65" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="66" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C66" s="5"/>
-      <c r="D66" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E66" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="F66" s="8" t="s">
+      <c r="F66" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="67" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C67" s="5"/>
+      <c r="C67" s="8"/>
       <c r="D67" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F67" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F67" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="68" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C68" s="5"/>
+      <c r="C68" s="8"/>
       <c r="D68" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E68" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="C69" s="8"/>
+      <c r="D69" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E69" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="F68" s="8" t="s">
+      <c r="F69" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C69" s="5"/>
-      <c r="D69" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E69" s="7" t="s">
+    <row r="70" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C70" s="8"/>
+      <c r="D70" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F69" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="70" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C70" s="5"/>
-      <c r="D70" s="6" t="s">
+      <c r="E70" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E70" s="11" t="s">
+      <c r="F70" s="11"/>
+    </row>
+    <row r="71" spans="3:6" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="C71" s="8" t="s">
         <v>94</v>
-      </c>
-      <c r="F70" s="11"/>
-    </row>
-    <row r="71" spans="3:6" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="C71" s="5" t="s">
-        <v>95</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F71" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F71" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="72" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C72" s="5"/>
+      <c r="C72" s="8"/>
       <c r="D72" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="F72" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F72" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="73" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C73" s="5"/>
+      <c r="C73" s="8"/>
       <c r="D73" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E73" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="74" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C74" s="8"/>
+      <c r="D74" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E74" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="F73" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="74" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C74" s="5"/>
-      <c r="D74" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E74" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F74" s="8" t="s">
+      <c r="F74" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="75" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C75" s="5"/>
+      <c r="C75" s="8"/>
       <c r="D75" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="F75" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F75" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="76" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C76" s="5"/>
+      <c r="C76" s="8"/>
       <c r="D76" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E76" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="3:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="C77" s="8"/>
+      <c r="D77" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E77" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F76" s="8" t="s">
+      <c r="F77" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="3:6" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C77" s="5"/>
-      <c r="D77" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E77" s="7" t="s">
+    <row r="78" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C78" s="8"/>
+      <c r="D78" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E78" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F77" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C78" s="5"/>
-      <c r="D78" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E78" s="9" t="s">
+      <c r="F78" s="9"/>
+    </row>
+    <row r="79" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="C79" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="F78" s="9"/>
-    </row>
-    <row r="79" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C79" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="D79" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="F79" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F79" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="80" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C80" s="5"/>
+      <c r="C80" s="8"/>
       <c r="D80" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F80" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F80" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="81" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C81" s="5"/>
+      <c r="C81" s="8"/>
       <c r="D81" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E81" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C82" s="8"/>
+      <c r="D82" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E82" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F81" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="82" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C82" s="5"/>
-      <c r="D82" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E82" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="F82" s="8" t="s">
+      <c r="F82" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="83" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C83" s="5"/>
+      <c r="C83" s="8"/>
       <c r="D83" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E83" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F83" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F83" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="84" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C84" s="5"/>
+      <c r="C84" s="8"/>
       <c r="D84" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E84" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="3:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="C85" s="8"/>
+      <c r="D85" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E85" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="F84" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="85" spans="3:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="C85" s="5"/>
-      <c r="D85" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E85" s="7" t="s">
+      <c r="F85" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C86" s="8"/>
+      <c r="D86" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E86" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F85" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="86" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C86" s="5"/>
-      <c r="D86" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E86" s="9" t="s">
+      <c r="F86" s="9"/>
+    </row>
+    <row r="87" spans="3:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="C87" s="8" t="s">
         <v>112</v>
-      </c>
-      <c r="F86" s="9"/>
-    </row>
-    <row r="87" spans="3:6" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C87" s="5" t="s">
-        <v>113</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="F87" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="F87" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="88" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C88" s="5"/>
+      <c r="C88" s="8"/>
       <c r="D88" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="F88" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="F88" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="89" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C89" s="5"/>
+      <c r="C89" s="8"/>
       <c r="D89" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E89" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="90" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C90" s="8"/>
+      <c r="D90" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E90" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="F89" s="8" t="s">
+      <c r="F90" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="90" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C90" s="5"/>
-      <c r="D90" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E90" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="F90" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
     <row r="91" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C91" s="5"/>
+      <c r="C91" s="8"/>
       <c r="D91" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="F91" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F91" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="92" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C92" s="5"/>
+      <c r="C92" s="8"/>
       <c r="D92" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E92" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="3:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="C93" s="8"/>
+      <c r="D93" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E93" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="F92" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="93" spans="3:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="C93" s="5"/>
-      <c r="D93" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E93" s="7" t="s">
+      <c r="F93" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C94" s="8"/>
+      <c r="D94" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E94" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="F93" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="94" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C94" s="5"/>
-      <c r="D94" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E94" s="9" t="s">
+      <c r="F94" s="9"/>
+    </row>
+    <row r="95" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="C95" s="8" t="s">
         <v>121</v>
-      </c>
-      <c r="F94" s="9"/>
-    </row>
-    <row r="95" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C95" s="5" t="s">
-        <v>122</v>
       </c>
       <c r="D95" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F95" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F95" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="96" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C96" s="5"/>
+      <c r="C96" s="8"/>
       <c r="D96" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E96" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="F96" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="F96" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="97" spans="3:6" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C97" s="5"/>
+      <c r="C97" s="8"/>
       <c r="D97" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E97" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="98" spans="3:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="C98" s="8"/>
+      <c r="D98" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E98" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="F97" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="98" spans="3:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="C98" s="5"/>
-      <c r="D98" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E98" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="F98" s="8" t="s">
+      <c r="F98" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="99" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C99" s="5"/>
+      <c r="C99" s="8"/>
       <c r="D99" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E99" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="F99" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F99" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="100" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C100" s="5"/>
+      <c r="C100" s="8"/>
       <c r="D100" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E100" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="C101" s="8"/>
+      <c r="D101" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E101" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="F100" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="101" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C101" s="5"/>
-      <c r="D101" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E101" s="7" t="s">
+      <c r="F101" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="102" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C102" s="8"/>
+      <c r="D102" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E102" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="F101" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="102" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C102" s="5"/>
-      <c r="D102" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E102" s="9" t="s">
+      <c r="F102" s="9"/>
+    </row>
+    <row r="103" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C103" s="8" t="s">
         <v>130</v>
-      </c>
-      <c r="F102" s="9"/>
-    </row>
-    <row r="103" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C103" s="5" t="s">
-        <v>131</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="F103" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="F103" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="104" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C104" s="5"/>
+      <c r="C104" s="8"/>
       <c r="D104" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="F104" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="F104" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="105" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C105" s="5"/>
+      <c r="C105" s="8"/>
       <c r="D105" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E105" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F105" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="106" spans="3:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="C106" s="8"/>
+      <c r="D106" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E106" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="F105" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="106" spans="3:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="C106" s="5"/>
-      <c r="D106" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E106" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="F106" s="8" t="s">
+      <c r="F106" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="107" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C107" s="5"/>
+      <c r="C107" s="8"/>
       <c r="D107" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="F107" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="F107" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="108" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C108" s="5"/>
+      <c r="C108" s="8"/>
       <c r="D108" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E108" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="C109" s="8"/>
+      <c r="D109" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E109" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="F108" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="109" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C109" s="5"/>
-      <c r="D109" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E109" s="7" t="s">
+      <c r="F109" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="110" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C110" s="8"/>
+      <c r="D110" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E110" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="F109" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="110" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C110" s="5"/>
-      <c r="D110" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E110" s="9" t="s">
+      <c r="F110" s="9"/>
+    </row>
+    <row r="111" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="C111" s="8" t="s">
         <v>139</v>
-      </c>
-      <c r="F110" s="9"/>
-    </row>
-    <row r="111" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C111" s="5" t="s">
-        <v>140</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E111" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F111" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="F111" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="112" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C112" s="5"/>
+      <c r="C112" s="8"/>
       <c r="D112" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E112" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="F112" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F112" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="113" spans="3:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="C113" s="5"/>
+      <c r="C113" s="8"/>
       <c r="D113" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E113" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="F113" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="114" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C114" s="8"/>
+      <c r="D114" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E114" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="F113" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="114" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C114" s="5"/>
-      <c r="D114" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E114" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="F114" s="8" t="s">
+      <c r="F114" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="115" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C115" s="5"/>
+      <c r="C115" s="8"/>
       <c r="D115" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E115" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="F115" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="F115" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="116" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C116" s="5"/>
+      <c r="C116" s="8"/>
       <c r="D116" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E116" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="F116" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="117" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="C117" s="8"/>
+      <c r="D117" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E117" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="F116" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="117" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C117" s="5"/>
-      <c r="D117" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E117" s="7" t="s">
+      <c r="F117" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="118" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C118" s="8"/>
+      <c r="D118" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E118" s="9" t="s">
         <v>147</v>
-      </c>
-      <c r="F117" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="118" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C118" s="5"/>
-      <c r="D118" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E118" s="9" t="s">
-        <v>148</v>
       </c>
       <c r="F118" s="9"/>
     </row>
     <row r="119" spans="3:6" ht="72" x14ac:dyDescent="0.3">
       <c r="C119" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D119" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E119" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="F119" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F119" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2503,9 +2503,9 @@
         <v>24</v>
       </c>
       <c r="E120" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="F120" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="F120" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2515,21 +2515,21 @@
         <v>8</v>
       </c>
       <c r="E121" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="F121" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="F121" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="122" spans="3:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="C122" s="10"/>
       <c r="D122" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E122" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="F122" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="F122" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2539,9 +2539,9 @@
         <v>13</v>
       </c>
       <c r="E123" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="F123" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="F123" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2551,652 +2551,652 @@
         <v>15</v>
       </c>
       <c r="E124" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="F124" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="F124" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="125" spans="3:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="C125" s="10"/>
       <c r="D125" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E125" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="F125" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="126" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+      <c r="F125" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="126" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C126" s="10"/>
       <c r="D126" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E126" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="F126" s="9"/>
+    </row>
+    <row r="127" spans="3:6" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="C127" s="8" t="s">
         <v>157</v>
-      </c>
-      <c r="F126" s="9"/>
-    </row>
-    <row r="127" spans="3:6" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="C127" s="5" t="s">
-        <v>158</v>
       </c>
       <c r="D127" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E127" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="F127" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="F127" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="128" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C128" s="5"/>
+      <c r="C128" s="8"/>
       <c r="D128" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E128" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="F128" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="F128" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="129" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C129" s="5"/>
+      <c r="C129" s="8"/>
       <c r="D129" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E129" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F129" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="130" spans="3:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="C130" s="8"/>
+      <c r="D130" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E130" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="F129" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="130" spans="3:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="C130" s="5"/>
-      <c r="D130" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E130" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="F130" s="8" t="s">
+      <c r="F130" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="131" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C131" s="5"/>
+      <c r="C131" s="8"/>
       <c r="D131" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E131" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="F131" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="F131" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="132" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C132" s="5"/>
+      <c r="C132" s="8"/>
       <c r="D132" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E132" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F132" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="133" spans="3:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="C133" s="8"/>
+      <c r="D133" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E133" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="F132" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="133" spans="3:6" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C133" s="5"/>
-      <c r="D133" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E133" s="7" t="s">
+      <c r="F133" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="134" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C134" s="8"/>
+      <c r="D134" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E134" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="F133" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="134" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C134" s="5"/>
-      <c r="D134" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E134" s="9" t="s">
+      <c r="F134" s="9"/>
+    </row>
+    <row r="135" spans="3:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="C135" s="8" t="s">
         <v>166</v>
-      </c>
-      <c r="F134" s="9"/>
-    </row>
-    <row r="135" spans="3:6" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C135" s="5" t="s">
-        <v>167</v>
       </c>
       <c r="D135" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E135" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="F135" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F135" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="136" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C136" s="5"/>
+      <c r="C136" s="8"/>
       <c r="D136" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E136" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="F136" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="F136" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="137" spans="3:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="C137" s="5"/>
+      <c r="C137" s="8"/>
       <c r="D137" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E137" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="F137" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="138" spans="3:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="C138" s="8"/>
+      <c r="D138" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E138" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="F137" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="138" spans="3:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="C138" s="5"/>
-      <c r="D138" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E138" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="F138" s="8" t="s">
+      <c r="F138" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="139" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C139" s="5"/>
+      <c r="C139" s="8"/>
       <c r="D139" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E139" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="F139" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="F139" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="140" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C140" s="5"/>
+      <c r="C140" s="8"/>
       <c r="D140" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E140" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="F140" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="141" spans="3:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="C141" s="8"/>
+      <c r="D141" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E141" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="F140" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="141" spans="3:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="C141" s="5"/>
-      <c r="D141" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E141" s="7" t="s">
+      <c r="F141" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="142" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C142" s="8"/>
+      <c r="D142" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E142" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="F141" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="142" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C142" s="5"/>
-      <c r="D142" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E142" s="9" t="s">
+      <c r="F142" s="9"/>
+    </row>
+    <row r="143" spans="3:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="C143" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="F142" s="9"/>
-    </row>
-    <row r="143" spans="3:6" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C143" s="5" t="s">
-        <v>176</v>
       </c>
       <c r="D143" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E143" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="F143" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="F143" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="144" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C144" s="5"/>
+      <c r="C144" s="8"/>
       <c r="D144" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E144" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="F144" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="F144" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="145" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C145" s="5"/>
+      <c r="C145" s="8"/>
       <c r="D145" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E145" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="F145" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="146" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="C146" s="8"/>
+      <c r="D146" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E146" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="F145" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="146" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C146" s="5"/>
-      <c r="D146" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E146" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="F146" s="8" t="s">
+      <c r="F146" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="147" spans="3:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="C147" s="5"/>
+      <c r="C147" s="8"/>
       <c r="D147" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E147" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="F147" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="F147" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="148" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C148" s="5"/>
+      <c r="C148" s="8"/>
       <c r="D148" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E148" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F148" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="149" spans="3:6" ht="67.2" x14ac:dyDescent="0.3">
+      <c r="C149" s="8"/>
+      <c r="D149" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E149" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="F148" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="149" spans="3:6" ht="67.2" x14ac:dyDescent="0.3">
-      <c r="C149" s="5"/>
-      <c r="D149" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E149" s="7" t="s">
+      <c r="F149" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="150" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C150" s="8"/>
+      <c r="D150" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E150" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="F149" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="150" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C150" s="5"/>
-      <c r="D150" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E150" s="9" t="s">
+      <c r="F150" s="9"/>
+    </row>
+    <row r="151" spans="3:6" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="C151" s="8" t="s">
         <v>184</v>
-      </c>
-      <c r="F150" s="9"/>
-    </row>
-    <row r="151" spans="3:6" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="C151" s="5" t="s">
-        <v>185</v>
       </c>
       <c r="D151" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E151" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="F151" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="F151" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="152" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C152" s="5"/>
+      <c r="C152" s="8"/>
       <c r="D152" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E152" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="F152" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="F152" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="153" spans="3:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="C153" s="5"/>
+      <c r="C153" s="8"/>
       <c r="D153" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E153" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="F153" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="154" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C154" s="8"/>
+      <c r="D154" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E154" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="F153" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="154" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C154" s="5"/>
-      <c r="D154" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E154" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="F154" s="8" t="s">
+      <c r="F154" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="155" spans="3:6" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C155" s="5"/>
+      <c r="C155" s="8"/>
       <c r="D155" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E155" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="F155" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="F155" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="156" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C156" s="5"/>
+      <c r="C156" s="8"/>
       <c r="D156" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E156" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F156" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="157" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C157" s="8"/>
+      <c r="D157" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E157" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="F156" s="8" t="s">
+      <c r="F157" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C157" s="5"/>
-      <c r="D157" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E157" s="7" t="s">
+    <row r="158" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C158" s="8"/>
+      <c r="D158" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E158" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="F157" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="158" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C158" s="5"/>
-      <c r="D158" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E158" s="9" t="s">
+      <c r="F158" s="9"/>
+    </row>
+    <row r="159" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="C159" s="8" t="s">
         <v>193</v>
-      </c>
-      <c r="F158" s="9"/>
-    </row>
-    <row r="159" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C159" s="5" t="s">
-        <v>194</v>
       </c>
       <c r="D159" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E159" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="F159" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="F159" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="160" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C160" s="5"/>
+      <c r="C160" s="8"/>
       <c r="D160" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E160" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="F160" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="F160" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="161" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C161" s="5"/>
+      <c r="C161" s="8"/>
       <c r="D161" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E161" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="F161" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C162" s="8"/>
+      <c r="D162" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E162" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="F161" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="162" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C162" s="5"/>
-      <c r="D162" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E162" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="F162" s="8" t="s">
+      <c r="F162" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="163" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C163" s="5"/>
+      <c r="C163" s="8"/>
       <c r="D163" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E163" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="F163" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F163" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="164" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C164" s="5"/>
+      <c r="C164" s="8"/>
       <c r="D164" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E164" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="F164" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="165" spans="3:6" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="C165" s="8"/>
+      <c r="D165" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E165" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="F164" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="165" spans="3:6" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="C165" s="5"/>
-      <c r="D165" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E165" s="7" t="s">
+      <c r="F165" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="166" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C166" s="8"/>
+      <c r="D166" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E166" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="F165" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="166" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C166" s="5"/>
-      <c r="D166" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E166" s="9" t="s">
+      <c r="F166" s="9"/>
+    </row>
+    <row r="167" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="C167" s="8" t="s">
         <v>202</v>
-      </c>
-      <c r="F166" s="9"/>
-    </row>
-    <row r="167" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C167" s="5" t="s">
-        <v>203</v>
       </c>
       <c r="D167" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E167" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="F167" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="F167" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="168" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C168" s="5"/>
+      <c r="C168" s="8"/>
       <c r="D168" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E168" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="F168" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="F168" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="169" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C169" s="5"/>
+      <c r="C169" s="8"/>
       <c r="D169" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E169" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="F169" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="170" spans="3:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="C170" s="8"/>
+      <c r="D170" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E170" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="F169" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="170" spans="3:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="C170" s="5"/>
-      <c r="D170" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E170" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="F170" s="8" t="s">
+      <c r="F170" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="171" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C171" s="5"/>
+      <c r="C171" s="8"/>
       <c r="D171" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E171" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="F171" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="F171" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="172" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C172" s="5"/>
+      <c r="C172" s="8"/>
       <c r="D172" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E172" s="7"/>
-      <c r="F172" s="8" t="s">
+      <c r="F172" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="173" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C173" s="5"/>
+      <c r="C173" s="8"/>
       <c r="D173" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E173" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="F173" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="174" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C174" s="8"/>
+      <c r="D174" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E174" s="9" t="s">
         <v>209</v>
-      </c>
-      <c r="F173" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="174" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C174" s="5"/>
-      <c r="D174" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E174" s="9" t="s">
-        <v>210</v>
       </c>
       <c r="F174" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="C7:C14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="C15:C22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="C23:C30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="C31:C38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="C39:C46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="C47:C54"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="C55:C62"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="C63:C70"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="C71:C78"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="C79:C86"/>
+    <mergeCell ref="E86:F86"/>
+    <mergeCell ref="C87:C94"/>
+    <mergeCell ref="E94:F94"/>
+    <mergeCell ref="C95:C102"/>
+    <mergeCell ref="E102:F102"/>
+    <mergeCell ref="C103:C110"/>
+    <mergeCell ref="E110:F110"/>
+    <mergeCell ref="C111:C118"/>
+    <mergeCell ref="E118:F118"/>
+    <mergeCell ref="C119:C126"/>
+    <mergeCell ref="E126:F126"/>
+    <mergeCell ref="C127:C134"/>
+    <mergeCell ref="E134:F134"/>
+    <mergeCell ref="C135:C142"/>
+    <mergeCell ref="E142:F142"/>
+    <mergeCell ref="C143:C150"/>
+    <mergeCell ref="E150:F150"/>
     <mergeCell ref="C151:C158"/>
     <mergeCell ref="E158:F158"/>
     <mergeCell ref="C159:C166"/>
     <mergeCell ref="E166:F166"/>
     <mergeCell ref="C167:C174"/>
     <mergeCell ref="E174:F174"/>
-    <mergeCell ref="C127:C134"/>
-    <mergeCell ref="E134:F134"/>
-    <mergeCell ref="C135:C142"/>
-    <mergeCell ref="E142:F142"/>
-    <mergeCell ref="C143:C150"/>
-    <mergeCell ref="E150:F150"/>
-    <mergeCell ref="C103:C110"/>
-    <mergeCell ref="E110:F110"/>
-    <mergeCell ref="C111:C118"/>
-    <mergeCell ref="E118:F118"/>
-    <mergeCell ref="C119:C126"/>
-    <mergeCell ref="E126:F126"/>
-    <mergeCell ref="C79:C86"/>
-    <mergeCell ref="E86:F86"/>
-    <mergeCell ref="C87:C94"/>
-    <mergeCell ref="E94:F94"/>
-    <mergeCell ref="C95:C102"/>
-    <mergeCell ref="E102:F102"/>
-    <mergeCell ref="C55:C62"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="C63:C70"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="C71:C78"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="C31:C38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="C39:C46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="C47:C54"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="C7:C14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="C15:C22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="C23:C30"/>
-    <mergeCell ref="E30:F30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated scoring EC3 score for Tella
</commit_message>
<xml_diff>
--- a/full_tool_evaluation_stylized.xlsx
+++ b/full_tool_evaluation_stylized.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amsuni-my.sharepoint.com/personal/james_bush_ii_student_uva_nl/Documents/thesis_final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{2081AC4A-61C1-478F-B65F-5C13FE051C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{996443BE-BC0F-41FE-9F1F-29355DD84D32}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{2081AC4A-61C1-478F-B65F-5C13FE051C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C82FEAB-1036-4C66-B4AD-B1B81F26C944}"/>
   <bookViews>
     <workbookView xWindow="45" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{2FDC8EDD-81E5-40A6-9283-0E9D69291070}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="212">
   <si>
     <t>Evaluations approved by tool's organization</t>
   </si>
@@ -682,7 +682,10 @@
     <t xml:space="preserve">USAID's Amazon Alive Activity, implemented by Chemonics, empowers indigenous communities in Colombia to monitor and safeguard their land, heritage, and rich biodiversity. Timby allows them to track and document potential threats to their territories, including illegal logging, mining, and land encroachment; while integrating their traditional knowledge, cultures, and ancestral ways of life and improving their decision-making processes (https://timby.org/case-studies/). </t>
   </si>
   <si>
-    <t>Automatically encrypts photos, videos, and audio recordings; All data being transferred between Tella and servers is encrypted through Transport Layer Security (TLS) (EC3.1); Files are pin/password protected; Captures verified metadata including a hash, but is not used to verify authenticity; Camouflage mode, quick delete panic button;</t>
+    <t>Automatically encrypts photos, videos, and audio recordings; All data being transferred between Tella and servers is encrypted through Transport Layer Security (TLS) (EC3.1); Files are pin/password protected; Captures verified metadata including a hash, but is not used to verify authenticity; Camouflage mode, quick delete panic button; * Role based access when connected with Uwazi, ODK (EC3.3) *;</t>
+  </si>
+  <si>
+    <t>No, * Partial when connected with Uwazi, ODK</t>
   </si>
 </sst>
 </file>
@@ -796,6 +799,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1118,7 +1125,7 @@
   <dimension ref="C5:F174"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="E17" sqref="E17:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1261,7 +1268,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="3:6" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="C17" s="10"/>
       <c r="D17" s="6" t="s">
         <v>8</v>
@@ -1270,7 +1277,7 @@
         <v>210</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>12</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3155,48 +3162,48 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="C151:C158"/>
+    <mergeCell ref="E158:F158"/>
+    <mergeCell ref="C159:C166"/>
+    <mergeCell ref="E166:F166"/>
+    <mergeCell ref="C167:C174"/>
+    <mergeCell ref="E174:F174"/>
+    <mergeCell ref="C127:C134"/>
+    <mergeCell ref="E134:F134"/>
+    <mergeCell ref="C135:C142"/>
+    <mergeCell ref="E142:F142"/>
+    <mergeCell ref="C143:C150"/>
+    <mergeCell ref="E150:F150"/>
+    <mergeCell ref="C103:C110"/>
+    <mergeCell ref="E110:F110"/>
+    <mergeCell ref="C111:C118"/>
+    <mergeCell ref="E118:F118"/>
+    <mergeCell ref="C119:C126"/>
+    <mergeCell ref="E126:F126"/>
+    <mergeCell ref="C79:C86"/>
+    <mergeCell ref="E86:F86"/>
+    <mergeCell ref="C87:C94"/>
+    <mergeCell ref="E94:F94"/>
+    <mergeCell ref="C95:C102"/>
+    <mergeCell ref="E102:F102"/>
+    <mergeCell ref="C55:C62"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="C63:C70"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="C71:C78"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="C31:C38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="C39:C46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="C47:C54"/>
+    <mergeCell ref="E54:F54"/>
     <mergeCell ref="C7:C14"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="C15:C22"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="C23:C30"/>
     <mergeCell ref="E30:F30"/>
-    <mergeCell ref="C31:C38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="C39:C46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="C47:C54"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="C55:C62"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="C63:C70"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="C71:C78"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="C79:C86"/>
-    <mergeCell ref="E86:F86"/>
-    <mergeCell ref="C87:C94"/>
-    <mergeCell ref="E94:F94"/>
-    <mergeCell ref="C95:C102"/>
-    <mergeCell ref="E102:F102"/>
-    <mergeCell ref="C103:C110"/>
-    <mergeCell ref="E110:F110"/>
-    <mergeCell ref="C111:C118"/>
-    <mergeCell ref="E118:F118"/>
-    <mergeCell ref="C119:C126"/>
-    <mergeCell ref="E126:F126"/>
-    <mergeCell ref="C127:C134"/>
-    <mergeCell ref="E134:F134"/>
-    <mergeCell ref="C135:C142"/>
-    <mergeCell ref="E142:F142"/>
-    <mergeCell ref="C143:C150"/>
-    <mergeCell ref="E150:F150"/>
-    <mergeCell ref="C151:C158"/>
-    <mergeCell ref="E158:F158"/>
-    <mergeCell ref="C159:C166"/>
-    <mergeCell ref="E166:F166"/>
-    <mergeCell ref="C167:C174"/>
-    <mergeCell ref="E174:F174"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>